<commit_message>
Add markdown versions of the excel files to facilitate online readability
</commit_message>
<xml_diff>
--- a/doc/SLR_results/results_of_investigation_on_PhD_theses.xlsx
+++ b/doc/SLR_results/results_of_investigation_on_PhD_theses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0-All-vscode-projects\2020-02-FLImpact work extension\rebuttal-tosem22\补充数据分析-R1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0-All-vscode-projects\2020-02-FLImpact work extension\rebuttal-tosem22\R2-小修\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B56490-F0BD-4F4E-B623-D4E093BF4174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27FAF1B-2E88-49CF-856D-06B916FADC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Ph.D. Dissertation</t>
   </si>
@@ -42,9 +42,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>It reported the "Patch correctness assessment bias 3" and "Patch correctness assessment bias 4", the same biases reported by Le et al. \cite{le2019reliability}.</t>
-  </si>
-  <si>
     <t>It reported the "Fault localization bias", the same biases reported by Liu et al. \cite{liu2019you}.</t>
   </si>
   <si>
@@ -137,6 +134,14 @@
   </si>
   <si>
     <t>Automatic software generation and improvement through search based techniques</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It reported the "Only-manual validation bias" and "Only-independent test validation bias", the same biases reported by Le et al. \cite{le2019reliability}.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -511,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -527,7 +532,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -547,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5">
         <v>2009</v>
@@ -564,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5">
         <v>2013</v>
@@ -581,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5">
         <v>2014</v>
@@ -598,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5">
         <v>2014</v>
@@ -615,13 +620,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5">
         <v>2015</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>4</v>
@@ -632,7 +637,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5">
         <v>2015</v>
@@ -649,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5">
         <v>2015</v>
@@ -666,7 +671,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5">
         <v>2015</v>
@@ -683,7 +688,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5">
         <v>2016</v>
@@ -700,7 +705,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5">
         <v>2017</v>
@@ -717,7 +722,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5">
         <v>2018</v>
@@ -734,7 +739,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5">
         <v>2018</v>
@@ -751,7 +756,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="5">
         <v>2018</v>
@@ -768,7 +773,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5">
         <v>2018</v>
@@ -785,22 +790,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="5">
         <v>2018</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="5">
         <v>2018</v>
@@ -817,7 +824,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="5">
         <v>2018</v>
@@ -834,13 +841,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="5">
         <v>2019</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>4</v>
@@ -851,7 +858,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5">
         <v>2019</v>
@@ -868,7 +875,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="5">
         <v>2020</v>
@@ -885,7 +892,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="5">
         <v>2020</v>

</xml_diff>